<commit_message>
improviments in the fault type library
</commit_message>
<xml_diff>
--- a/feasibility-study/comparation-ccsl-vs-pmd.xlsx
+++ b/feasibility-study/comparation-ccsl-vs-pmd.xlsx
@@ -8,32 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repositories\Coding-Conventions-Specification-Language\feasibility-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F326C8F9-BD9E-4C1D-82AC-7ADBCFA81C4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194ABA80-0F59-4EAC-98E1-B6E20C1C7ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PMD vs. CCSL" sheetId="1" r:id="rId1"/>
-    <sheet name="Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Apache Commons Collections" sheetId="1" r:id="rId1"/>
+    <sheet name="Commons Collections (Details)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
   <si>
     <t>PMD Rule Id</t>
   </si>
   <si>
-    <t>category/java/performance.xml/AppendCharacterWithChar</t>
-  </si>
-  <si>
     <t>PMD Rule Name</t>
   </si>
   <si>
@@ -49,9 +51,6 @@
     <t>AddEmptyString</t>
   </si>
   <si>
-    <t>category/java/performance.xml/AddEmptyString</t>
-  </si>
-  <si>
     <t>fix getting all statements of a InfixExpression</t>
   </si>
   <si>
@@ -61,9 +60,6 @@
     <t>#CCSL Matches</t>
   </si>
   <si>
-    <t>category/java/performance.xml/AvoidFileStream</t>
-  </si>
-  <si>
     <t>AvoidFileStream</t>
   </si>
   <si>
@@ -73,33 +69,15 @@
     <t>#CCSL Violations Files</t>
   </si>
   <si>
-    <t>category/java/performance.xml/AvoidUsingShortType</t>
-  </si>
-  <si>
     <t>AvoidUsingShortType</t>
   </si>
   <si>
-    <t>category/java/performance.xml/BigIntegerInstantiation</t>
-  </si>
-  <si>
     <t>BooleanInstantiation</t>
   </si>
   <si>
-    <t>category/java/performance.xml/BooleanInstantiation</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/ByteInstantiation</t>
-  </si>
-  <si>
     <t>ByteInstantiation</t>
   </si>
   <si>
-    <t>category/java/performance.xml/InefficientEmptyStringCheck</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/IntegerInstantiation</t>
-  </si>
-  <si>
     <t>IntegerInstantiation</t>
   </si>
   <si>
@@ -115,9 +93,6 @@
     <t>BigIntegerInstantiation</t>
   </si>
   <si>
-    <t>category/java/performance.xml/LongInstantiation</t>
-  </si>
-  <si>
     <t>LongInstantiation</t>
   </si>
   <si>
@@ -152,9 +127,6 @@
   </si>
   <si>
     <t>RedundantFieldInitializer</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/RedundantFieldInitializer</t>
   </si>
   <si>
     <t>#CCSL False Positives</t>
@@ -183,13 +155,7 @@
     <t>ShortInstantiation</t>
   </si>
   <si>
-    <t>category/java/performance.xml/ShortInstantiation</t>
-  </si>
-  <si>
     <t>SimplifyStartsWith</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/SimplifyStartsWith</t>
   </si>
   <si>
     <t>src\test\java\org\apache\commons\collections4\set\PredicatedNavigableSetTest.java:65
@@ -197,9 +163,6 @@
   </si>
   <si>
     <t>StringInstantiation</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/StringInstantiation</t>
   </si>
   <si>
     <t>src\test\java\org\apache\commons\collections4\list\SetUniqueListTest.java:63
@@ -224,27 +187,15 @@
     <t>StringToString</t>
   </si>
   <si>
-    <t>category/java/performance.xml/StringToString</t>
-  </si>
-  <si>
     <t>TooFewBranchesForASwitchStatement</t>
   </si>
   <si>
-    <t>category/java/performance.xml/TooFewBranchesForASwitchStatement</t>
-  </si>
-  <si>
     <t>UnnecessaryWrapperObjectCreation</t>
   </si>
   <si>
-    <t>category/java/performance.xml/UnnecessaryWrapperObjectCreation</t>
-  </si>
-  <si>
     <t>UseArrayListInsteadOfVector</t>
   </si>
   <si>
-    <t>category/java/performance.xml/UseArrayListInsteadOfVector</t>
-  </si>
-  <si>
     <t>UseArraysAsList</t>
   </si>
   <si>
@@ -263,32 +214,62 @@
     <t>PMD False Negatives</t>
   </si>
   <si>
-    <t>category/java/performance.xml/UseIndexOfChar</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/UselessStringValueOf</t>
-  </si>
-  <si>
     <t>UseStringBufferForStringAppends</t>
   </si>
   <si>
-    <t>category/java/performance.xml/UseStringBufferForStringAppends</t>
-  </si>
-  <si>
     <t>UseStringBufferLength</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/UseStringBufferLength</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/InefficientStringBuffering</t>
-  </si>
-  <si>
-    <t>category/java/performance.xml/InsufficientStringBufferDeclaration</t>
   </si>
   <si>
     <t>src\test\java\org\apache\commons\collections4\IterableUtilsTest.java:94
 src\test\java\org\apache\commons\collections4\IterableUtilsTest.java:96</t>
+  </si>
+  <si>
+    <t>Insufficient Results</t>
+  </si>
+  <si>
+    <t>Legenda:</t>
+  </si>
+  <si>
+    <t>Excellent (CCSL has found more than PMD)</t>
+  </si>
+  <si>
+    <t>Difficult Rules</t>
+  </si>
+  <si>
+    <t>Partial Results (CCSL has found less than PMD)</t>
+  </si>
+  <si>
+    <t>AvoidSynchronizedAtMethodLevel</t>
+  </si>
+  <si>
+    <t>AvoidThreadGroup</t>
+  </si>
+  <si>
+    <t>AvoidUsingVolatile</t>
+  </si>
+  <si>
+    <t>DoNotUseThreads</t>
+  </si>
+  <si>
+    <t>DontCallThreadRun</t>
+  </si>
+  <si>
+    <t>DoubleCheckedLocking</t>
+  </si>
+  <si>
+    <t>NonThreadSafeSingleton</t>
+  </si>
+  <si>
+    <t>UnsynchronizedStaticDateFormatter</t>
+  </si>
+  <si>
+    <t>UnsynchronizedStaticFormatter</t>
+  </si>
+  <si>
+    <t>UseConcurrentHashMap</t>
+  </si>
+  <si>
+    <t>UseNotifyAllInsteadOfNotify</t>
   </si>
 </sst>
 </file>
@@ -310,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +322,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -354,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,6 +367,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,13 +650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A2:A31"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,52 +671,59 @@
     <col min="8" max="9" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="53.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="79.6640625" customWidth="1"/>
-    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="53.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f t="shared" ref="B2:B31" si="0">CONCATENATE("category/java/performance.xml/", A2)</f>
+        <v>category/java/performance.xml/AddEmptyString</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -738,18 +747,22 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/AppendCharacterWithChar</v>
       </c>
       <c r="C3" s="2">
         <v>12</v>
@@ -773,17 +786,23 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/AvoidArrayLoops</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -793,13 +812,17 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/AvoidFileStream</v>
       </c>
       <c r="C5" s="4">
         <v>7</v>
@@ -823,17 +846,23 @@
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/AvoidInstantiatingObjectsInLoops</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -844,12 +873,13 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/AvoidUsingShortType</v>
       </c>
       <c r="C7" s="2">
         <v>5</v>
@@ -873,16 +903,17 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/BigIntegerInstantiation</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -890,13 +921,32 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/BooleanInstantiation</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
@@ -920,16 +970,17 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/ByteInstantiation</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -953,15 +1004,18 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/ConsecutiveAppendsShouldReuse</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -972,11 +1026,14 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/ConsecutiveLiteralAppends</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -987,12 +1044,13 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/InefficientEmptyStringCheck</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1015,13 +1073,17 @@
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>75</v>
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/InefficientStringBuffering</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1029,13 +1091,32 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/InsufficientStringBufferDeclaration</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1047,12 +1128,13 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/IntegerInstantiation</v>
       </c>
       <c r="C16" s="4">
         <v>9</v>
@@ -1076,18 +1158,19 @@
         <v>0</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/LongInstantiation</v>
       </c>
       <c r="C17" s="2">
         <v>10</v>
@@ -1105,15 +1188,18 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/OptimizableToArrayCall</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1126,10 +1212,11 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/RedundantFieldInitializer</v>
       </c>
       <c r="C19" s="4">
         <v>144</v>
@@ -1153,18 +1240,19 @@
         <v>0</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/ShortInstantiation</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -1188,16 +1276,17 @@
         <v>0</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/SimplifyStartsWith</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
@@ -1219,51 +1308,53 @@
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="A22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/StringInstantiation</v>
+      </c>
+      <c r="C22" s="9">
         <v>6</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="9">
         <v>2</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="9">
         <v>23</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="9">
         <v>7</v>
       </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
         <v>17</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="2"/>
+      <c r="J22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
+      <c r="A23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/StringToString</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1274,10 +1365,11 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/TooFewBranchesForASwitchStatement</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -1301,16 +1393,17 @@
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="B25" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UnnecessaryWrapperObjectCreation</v>
       </c>
       <c r="C25" s="8">
         <v>0</v>
@@ -1336,10 +1429,11 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UseArrayListInsteadOfVector</v>
       </c>
       <c r="C26" s="2">
         <v>6</v>
@@ -1363,15 +1457,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="B27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UseArraysAsList</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1384,10 +1481,11 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>46</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UseIndexOfChar</v>
       </c>
       <c r="C28" s="2">
         <v>3</v>
@@ -1411,16 +1509,17 @@
         <v>0</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UselessStringValueOf</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -1444,16 +1543,17 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>72</v>
+      <c r="A30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UseStringBufferForStringAppends</v>
       </c>
       <c r="C30" s="8">
         <v>0</v>
@@ -1463,17 +1563,183 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>74</v>
+      <c r="A31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>category/java/performance.xml/UseStringBufferLength</v>
       </c>
       <c r="C31" s="8">
         <v>0</v>
       </c>
       <c r="D31" s="8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f t="shared" ref="B33:B43" si="1">CONCATENATE("category/java/multithreading.xml/", A33)</f>
+        <v>category/java/multithreading.xml/AvoidSynchronizedAtMethodLevel</v>
+      </c>
+      <c r="C33" s="2">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2">
+        <v>7</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/AvoidThreadGroup</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/AvoidUsingVolatile</v>
+      </c>
+      <c r="C35" s="2">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/DoNotUseThreads</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/DontCallThreadRun</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/DoubleCheckedLocking</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/NonThreadSafeSingleton</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/UnsynchronizedStaticDateFormatter</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/UnsynchronizedStaticFormatter</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/UseConcurrentHashMap</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="1"/>
+        <v>category/java/multithreading.xml/UseNotifyAllInsteadOfNotify</v>
       </c>
     </row>
   </sheetData>
@@ -1486,11 +1752,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E851DE-B745-4A19-B57A-354113B40F15}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,178 +1769,178 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>